<commit_message>
Answered 4 answers of 1.1 by consider appropriate encoding in R script
</commit_message>
<xml_diff>
--- a/Investment-case-study-group-project/Investments.xlsx
+++ b/Investment-case-study-group-project/Investments.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suresh.balla/Projects/data-science/Investment-case-study-group-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suresh.balla/Projects/data-science/GitHub/Investment-case-study-group-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7080"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>C1</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t>company_permalink</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -994,7 +997,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1042,7 +1045,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="17">
-        <v>90247</v>
+        <v>66368</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1074,7 +1077,9 @@
       <c r="B8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="17" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5">

</xml_diff>

<commit_message>
Completed section 1.1 questions
</commit_message>
<xml_diff>
--- a/Investment-case-study-group-project/Investments.xlsx
+++ b/Investment-case-study-group-project/Investments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16080"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -997,7 +997,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1088,7 +1088,9 @@
       <c r="B9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="17">
+        <v>114949</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="11"/>

</xml_diff>

<commit_message>
Section 1.1 questions in progress
</commit_message>
<xml_diff>
--- a/Investment-case-study-group-project/Investments.xlsx
+++ b/Investment-case-study-group-project/Investments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16080"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -996,7 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -1121,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1167,7 +1167,9 @@
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12">
+        <v>11748949.1</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
@@ -1176,7 +1178,9 @@
       <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="12">
+        <v>958694.5</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
@@ -1185,7 +1189,9 @@
       <c r="B7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="12">
+        <v>719818</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
@@ -1194,7 +1200,9 @@
       <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="12">
+        <v>73308593</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12">

</xml_diff>

<commit_message>
Completed checkpoint 3 - country analysis
</commit_message>
<xml_diff>
--- a/Investment-case-study-group-project/Investments.xlsx
+++ b/Investment-case-study-group-project/Investments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>C1</t>
   </si>
@@ -363,6 +363,18 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>post_ipo_debt?</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
   </si>
 </sst>
 </file>
@@ -1121,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1211,7 +1223,9 @@
       <c r="B9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1237,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1283,7 +1297,9 @@
       <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
@@ -1292,7 +1308,9 @@
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
@@ -1301,7 +1319,9 @@
       <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Updated R code and solution based on given constraint
</commit_message>
<xml_diff>
--- a/Investment-case-study-group-project/Investments.xlsx
+++ b/Investment-case-study-group-project/Investments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -365,16 +365,16 @@
     <t>N</t>
   </si>
   <si>
-    <t>post_ipo_debt?</t>
-  </si>
-  <si>
     <t>United States of America</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>New Zealand</t>
+    <t>venture</t>
+  </si>
+  <si>
+    <t>United Kingdom of Great Britain and Northern Ireland</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1134,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1224,7 +1224,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1252,14 +1252,14 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.1640625" customWidth="1"/>
     <col min="2" max="2" width="47.1640625" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="41.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1298,7 +1298,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Solution for Checkpoint 5: Sector Analysis 2
</commit_message>
<xml_diff>
--- a/Investment-case-study-group-project/Investments.xlsx
+++ b/Investment-case-study-group-project/Investments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>C1</t>
   </si>
@@ -375,6 +375,15 @@
   </si>
   <si>
     <t>India</t>
+  </si>
+  <si>
+    <t>Cleantech / Semiconductors</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Social, Finance, Analytics, Advertising</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1346,17 +1355,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="56.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="28.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1424,9 +1432,15 @@
       <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="C7" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="19">
@@ -1435,9 +1449,15 @@
       <c r="B8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
+      <c r="C8" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="19">

</xml_diff>

<commit_message>
Integrated deepak's other solutions (sql way querying) and update table 5.1 resutls
</commit_message>
<xml_diff>
--- a/Investment-case-study-group-project/Investments.xlsx
+++ b/Investment-case-study-group-project/Investments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" activeTab="3"/>
+    <workbookView xWindow="3640" yWindow="2660" windowWidth="24380" windowHeight="10800" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>C1</t>
   </si>
@@ -359,9 +359,6 @@
     <t>Sector-wise Investment Analysis</t>
   </si>
   <si>
-    <t>company_permalink</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -384,13 +381,22 @@
   </si>
   <si>
     <t>Social, Finance, Analytics, Advertising</t>
+  </si>
+  <si>
+    <t>permalink</t>
+  </si>
+  <si>
+    <t>News, Search and Messaging</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,6 +465,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -597,10 +610,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -701,8 +715,20 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1018,7 +1044,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1088,7 +1114,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1099,7 +1125,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1143,7 +1169,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1188,7 +1214,7 @@
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="36">
         <v>11748949.1</v>
       </c>
     </row>
@@ -1199,7 +1225,7 @@
       <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="36">
         <v>958694.5</v>
       </c>
     </row>
@@ -1210,7 +1236,7 @@
       <c r="B7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="36">
         <v>719818</v>
       </c>
     </row>
@@ -1221,7 +1247,7 @@
       <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="36">
         <v>73308593</v>
       </c>
     </row>
@@ -1233,7 +1259,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1307,7 +1333,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1318,7 +1344,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1329,7 +1355,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1356,14 +1382,14 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="56.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="40" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="28.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1372,10 +1398,12 @@
         <v>34</v>
       </c>
       <c r="B1" s="31"/>
+      <c r="C1" s="37"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="32"/>
       <c r="B2" s="33"/>
+      <c r="C2" s="37"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
@@ -1393,7 +1421,7 @@
       <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="38" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="23" t="s">
@@ -1410,9 +1438,15 @@
       <c r="B5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
+      <c r="C5" s="39">
+        <v>38372</v>
+      </c>
+      <c r="D5" s="17">
+        <v>2303</v>
+      </c>
+      <c r="E5" s="17">
+        <v>992</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="19">
@@ -1421,9 +1455,15 @@
       <c r="B6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="C6" s="39">
+        <v>422510842796</v>
+      </c>
+      <c r="D6" s="17">
+        <v>20245627416</v>
+      </c>
+      <c r="E6" s="17">
+        <v>14391858718</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="19">
@@ -1432,14 +1472,14 @@
       <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>47</v>
+      <c r="C7" s="39" t="s">
+        <v>46</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1449,14 +1489,14 @@
       <c r="B8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>46</v>
+      <c r="C8" s="39" t="s">
+        <v>45</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1466,9 +1506,15 @@
       <c r="B9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
+      <c r="C9" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
@@ -1477,9 +1523,15 @@
       <c r="B10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="C10" s="39">
+        <v>24853</v>
+      </c>
+      <c r="D10" s="17">
+        <v>580</v>
+      </c>
+      <c r="E10" s="17">
+        <v>332</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="19">
@@ -1488,9 +1540,15 @@
       <c r="B11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="C11" s="39">
+        <v>8268</v>
+      </c>
+      <c r="D11" s="17">
+        <v>481</v>
+      </c>
+      <c r="E11" s="17">
+        <v>193</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="19">
@@ -1499,9 +1557,15 @@
       <c r="B12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="C12" s="39">
+        <v>7822</v>
+      </c>
+      <c r="D12" s="17">
+        <v>466</v>
+      </c>
+      <c r="E12" s="17">
+        <v>154</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="19">
@@ -1510,7 +1574,7 @@
       <c r="B13" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="17"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
     </row>
@@ -1521,7 +1585,7 @@
       <c r="B14" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="39"/>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
     </row>

</xml_diff>

<commit_message>
Solution and results for sl.no 8 and 9 in table 5.1 and updated table 5.1 resutls
</commit_message>
<xml_diff>
--- a/Investment-case-study-group-project/Investments.xlsx
+++ b/Investment-case-study-group-project/Investments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="2660" windowWidth="24380" windowHeight="10800" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t>C1</t>
   </si>
@@ -387,6 +387,24 @@
   </si>
   <si>
     <t>News, Search and Messaging</t>
+  </si>
+  <si>
+    <t>/organization/social-finance</t>
+  </si>
+  <si>
+    <t>/organization/oneweb</t>
+  </si>
+  <si>
+    <t>/organization/flipkart</t>
+  </si>
+  <si>
+    <t>/organization/freescale</t>
+  </si>
+  <si>
+    <t>/organization/powa-technologies</t>
+  </si>
+  <si>
+    <t>/organization/shopclues-com</t>
   </si>
 </sst>
 </file>
@@ -682,6 +700,17 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -715,17 +744,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1055,23 +1073,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="30"/>
       <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -1180,21 +1198,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="32"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
     </row>
     <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -1214,7 +1232,7 @@
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="25">
         <v>11748949.1</v>
       </c>
     </row>
@@ -1225,7 +1243,7 @@
       <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="25">
         <v>958694.5</v>
       </c>
     </row>
@@ -1236,7 +1254,7 @@
       <c r="B7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="25">
         <v>719818</v>
       </c>
     </row>
@@ -1247,7 +1265,7 @@
       <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="25">
         <v>73308593</v>
       </c>
     </row>
@@ -1298,21 +1316,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="32"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -1382,37 +1400,37 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="56.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="28.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="37"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="37"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="26"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
@@ -1421,7 +1439,7 @@
       <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="27" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="23" t="s">
@@ -1438,7 +1456,7 @@
       <c r="B5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="28">
         <v>38372</v>
       </c>
       <c r="D5" s="17">
@@ -1455,7 +1473,7 @@
       <c r="B6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="28">
         <v>422510842796</v>
       </c>
       <c r="D6" s="17">
@@ -1472,7 +1490,7 @@
       <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="28" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="17" t="s">
@@ -1489,7 +1507,7 @@
       <c r="B8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="28" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="17" t="s">
@@ -1506,7 +1524,7 @@
       <c r="B9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="28" t="s">
         <v>47</v>
       </c>
       <c r="D9" s="17" t="s">
@@ -1523,7 +1541,7 @@
       <c r="B10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10" s="28">
         <v>24853</v>
       </c>
       <c r="D10" s="17">
@@ -1540,7 +1558,7 @@
       <c r="B11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="39">
+      <c r="C11" s="28">
         <v>8268</v>
       </c>
       <c r="D11" s="17">
@@ -1557,7 +1575,7 @@
       <c r="B12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="39">
+      <c r="C12" s="28">
         <v>7822</v>
       </c>
       <c r="D12" s="17">
@@ -1574,9 +1592,15 @@
       <c r="B13" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="C13" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
@@ -1585,9 +1609,15 @@
       <c r="B14" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="C14" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Updated R code and excel results based on clarifiactions from deepka with respect to filtering range for investments
</commit_message>
<xml_diff>
--- a/Investment-case-study-group-project/Investments.xlsx
+++ b/Investment-case-study-group-project/Investments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" activeTab="3"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16200" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -389,22 +389,22 @@
     <t>News, Search and Messaging</t>
   </si>
   <si>
-    <t>/organization/social-finance</t>
-  </si>
-  <si>
-    <t>/organization/oneweb</t>
-  </si>
-  <si>
-    <t>/organization/flipkart</t>
-  </si>
-  <si>
-    <t>/organization/freescale</t>
-  </si>
-  <si>
-    <t>/organization/powa-technologies</t>
-  </si>
-  <si>
-    <t>/organization/shopclues-com</t>
+    <t>Virtustream</t>
+  </si>
+  <si>
+    <t>Electric Cloud</t>
+  </si>
+  <si>
+    <t>FirstCry.com</t>
+  </si>
+  <si>
+    <t>Celltick Technologies</t>
+  </si>
+  <si>
+    <t>Manthan Systems</t>
+  </si>
+  <si>
+    <t>SST Inc. (Formerly ShotSpotter)</t>
   </si>
 </sst>
 </file>
@@ -632,7 +632,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -703,14 +703,7 @@
     <xf numFmtId="43" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -744,6 +737,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1073,23 +1074,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="27"/>
       <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -1198,21 +1199,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
     </row>
     <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -1316,21 +1317,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -1400,37 +1401,37 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="56.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" style="41" customWidth="1"/>
     <col min="4" max="5" width="28.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="38"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="26"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
@@ -1439,7 +1440,7 @@
       <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="39" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="23" t="s">
@@ -1456,14 +1457,14 @@
       <c r="B5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="28">
-        <v>38372</v>
+      <c r="C5" s="40">
+        <v>12150</v>
       </c>
       <c r="D5" s="17">
-        <v>2303</v>
+        <v>628</v>
       </c>
       <c r="E5" s="17">
-        <v>992</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1473,14 +1474,14 @@
       <c r="B6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="28">
-        <v>422510842796</v>
+      <c r="C6" s="26">
+        <v>108531347515</v>
       </c>
       <c r="D6" s="17">
-        <v>20245627416</v>
+        <v>5436843539</v>
       </c>
       <c r="E6" s="17">
-        <v>14391858718</v>
+        <v>2976543602</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1490,7 +1491,7 @@
       <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="40" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="17" t="s">
@@ -1507,8 +1508,8 @@
       <c r="B8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>45</v>
+      <c r="C8" s="40" t="s">
+        <v>47</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>47</v>
@@ -1524,8 +1525,8 @@
       <c r="B9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="28" t="s">
-        <v>47</v>
+      <c r="C9" s="40" t="s">
+        <v>45</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>45</v>
@@ -1541,14 +1542,14 @@
       <c r="B10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="28">
-        <v>24853</v>
+      <c r="C10" s="40">
+        <v>2950</v>
       </c>
       <c r="D10" s="17">
-        <v>580</v>
+        <v>147</v>
       </c>
       <c r="E10" s="17">
-        <v>332</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1558,14 +1559,14 @@
       <c r="B11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="28">
-        <v>8268</v>
+      <c r="C11" s="40">
+        <v>2714</v>
       </c>
       <c r="D11" s="17">
-        <v>481</v>
+        <v>133</v>
       </c>
       <c r="E11" s="17">
-        <v>193</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1575,14 +1576,14 @@
       <c r="B12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="28">
-        <v>7822</v>
+      <c r="C12" s="40">
+        <v>2350</v>
       </c>
       <c r="D12" s="17">
-        <v>466</v>
+        <v>130</v>
       </c>
       <c r="E12" s="17">
-        <v>154</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.2">
@@ -1592,7 +1593,7 @@
       <c r="B13" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="40" t="s">
         <v>50</v>
       </c>
       <c r="D13" s="17" t="s">
@@ -1609,14 +1610,14 @@
       <c r="B14" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="E14" s="17" t="s">
         <v>54</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>